<commit_message>
Added requirements from meeting 02/21/22
</commit_message>
<xml_diff>
--- a/Documents/TeamMeetings.xlsx
+++ b/Documents/TeamMeetings.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -40,18 +40,25 @@
     <t>Harrison, Nick, Jacob, Daniel</t>
   </si>
   <si>
-    <t>Total Minutes:</t>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Harrison, Nick, Jacob, Daniel, Brian</t>
+  </si>
+  <si>
+    <t>Total Time:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="h:mm am/pm"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -60,19 +67,13 @@
     <font>
       <b/>
       <sz val="12.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -115,7 +116,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="46" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="46" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -124,17 +125,27 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="46" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="46" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -387,7 +398,7 @@
         <v>0.5486111111111112</v>
       </c>
       <c r="D2" s="5">
-        <f>ABS(B2-C2)</f>
+        <f t="shared" ref="D2:D3" si="1">ABS(B2-C2)</f>
         <v>0.04861111111</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -398,152 +409,165 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="A3" s="8">
+        <v>44613.0</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.6923611111111111</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.6965277777777777</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.004166666667</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="10"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="14">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="16">
         <f>SUM(D2:D19)</f>
-        <v>0.04861111111</v>
+        <v>0.05277777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>